<commit_message>
EDA project 25-05 I
</commit_message>
<xml_diff>
--- a/Entregables/09_Proyecto Análisis/Modelo de datos deseado.xlsx
+++ b/Entregables/09_Proyecto Análisis/Modelo de datos deseado.xlsx
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F4:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>